<commit_message>
DOCS: Sistema Saldo Crédito completo + limpieza workspace
- Nueva documentación maestra: docs/SISTEMA_SALDO_CREDITO.md
  * Arquitectura completa con diagramas
  * Endpoints detallados con ejemplos
  * Guía de uso y mantenimiento
  * Troubleshooting común

- Actualización README.md principal
  * Agregar Sistema Saldo Crédito a características
  * Actualizar sección importación de datos
  * URLs de producción actuales
  * Referencias a nueva documentación

- Limpieza de workspace (60 archivos .md)
  * Movidos a docs/archive/ con README explicativo
  * Documentación obsoleta de sesiones previas
  * Estados intermedios y correcciones antiguas
  * Mantiene solo CREDENCIALES.md en raíz

Sistema completamente documentado y workspace limpio ✨
</commit_message>
<xml_diff>
--- a/docs/ARCHIVOS DE IMPORTACION/ARCHIVOS DE CARGA PERIODICA/SALDO CREDITO.xlsx
+++ b/docs/ARCHIVOS DE IMPORTACION/ARCHIVOS DE CARGA PERIODICA/SALDO CREDITO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariolabbe/Desktop/TRABAJO IA/CRM2/docs/ARCHIVOS DE IMPORTACION/ARCHIVOS DE CARGA PERIODICA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51FBBDBB-17A9-5F40-B659-AECFCFF680BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC822639-7C3C-F241-A4CA-28142DE9208C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="620" windowWidth="28800" windowHeight="16220" xr2:uid="{A7E44181-EA45-5744-B5F6-F3F662DF5E5F}"/>
   </bookViews>
@@ -5234,9 +5234,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C71681F1-C23F-374C-9387-CCDFEB233F78}">
   <dimension ref="A1:K1561"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>